<commit_message>
Added changes to Purchase List.xlsx
</commit_message>
<xml_diff>
--- a/Purchase List.xlsx
+++ b/Purchase List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Purchase List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Holed Mirror Translation</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Aline</t>
   </si>
   <si>
-    <t>Filter (Phosphor or Lanex)</t>
-  </si>
-  <si>
     <t>Find it or buy it! (Might be at Greque)</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t xml:space="preserve">Window Flange </t>
   </si>
   <si>
-    <t>For SH Wavefront Sensor</t>
-  </si>
-  <si>
     <t>Ceramic Plates</t>
   </si>
   <si>
@@ -106,14 +100,77 @@
     <t>ISO-K Tee + 2 Flanges</t>
   </si>
   <si>
-    <t>Size?</t>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Not ordered</t>
+  </si>
+  <si>
+    <t>Filter ( Lanex)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO 160 - </t>
+  </si>
+  <si>
+    <t>Quote requested 28/01/2015</t>
+  </si>
+  <si>
+    <t>For SH Wavefront Sensor : what coating?</t>
+  </si>
+  <si>
+    <t>Newport</t>
+  </si>
+  <si>
+    <t>Not ordered/not found</t>
+  </si>
+  <si>
+    <t>Vacuum-compatible subd 15 cable</t>
+  </si>
+  <si>
+    <t>3 metres</t>
+  </si>
+  <si>
+    <t>Quote requested 27/01/2015</t>
+  </si>
+  <si>
+    <t>Design not started</t>
+  </si>
+  <si>
+    <t>Verify stock + check with Benoit for what has already been ordered</t>
+  </si>
+  <si>
+    <t>Translation/flip for Beam block</t>
+  </si>
+  <si>
+    <t>Not designed</t>
+  </si>
+  <si>
+    <t>Shutter connector</t>
+  </si>
+  <si>
+    <t>Do we have everything?</t>
+  </si>
+  <si>
+    <t>Conformité ligne PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the performance of the translation stage up to specs? </t>
+  </si>
+  <si>
+    <t>Not done</t>
+  </si>
+  <si>
+    <t>1.5" mirror mounts</t>
+  </si>
+  <si>
+    <t>Add wedge to addtenuator design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,13 +178,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -142,8 +240,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -162,7 +276,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -204,7 +318,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,10 +350,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,7 +384,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -447,54 +559,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
@@ -503,9 +626,12 @@
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
@@ -514,126 +640,256 @@
       <c r="C8">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E8" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>26</v>
+      <c r="E10" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
+        <v>10</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="51.75" customHeight="1">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>14</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" ht="21" customHeight="1">
+      <c r="A21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22">
+      <c r="C23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
+      <c r="E23" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25">
+      <c r="E24" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="E26" s="3" t="s">
         <v>29</v>
       </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
+      <c r="E27" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="24.75" customHeight="1">
+      <c r="A30" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>